<commit_message>
Updated By 6.20 Time
</commit_message>
<xml_diff>
--- a/TestData/ComplianceSheet.xlsx
+++ b/TestData/ComplianceSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="6684" tabRatio="526" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="6684" tabRatio="526" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -733,10 +733,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -767,6 +767,9 @@
       <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="B4" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -829,7 +832,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update On 3005 time 10pm
</commit_message>
<xml_diff>
--- a/TestData/ComplianceSheet.xlsx
+++ b/TestData/ComplianceSheet.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LicenseManagement-main\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="6684" tabRatio="526" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="6684" tabRatio="526" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,6 +16,7 @@
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:D21"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -616,7 +612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -832,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>